<commit_message>
fix bug of QueueManager
</commit_message>
<xml_diff>
--- a/excel_file/specificBill.xlsx
+++ b/excel_file/specificBill.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="190">
   <si>
     <t>User ID</t>
   </si>
@@ -192,6 +192,396 @@
   </si>
   <si>
     <t>2.5</t>
+  </si>
+  <si>
+    <t>2024-05-23 10:34:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 10:34:52</t>
+  </si>
+  <si>
+    <t>2024-05-23 10:47:57</t>
+  </si>
+  <si>
+    <t>39.5</t>
+  </si>
+  <si>
+    <t>2024-05-03 20:00:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:50:23</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:53:15</t>
+  </si>
+  <si>
+    <t>45.5</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:56:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:56:12</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:59:43</t>
+  </si>
+  <si>
+    <t>56.5</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:59:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:59:52</t>
+  </si>
+  <si>
+    <t>2024-05-23 15:59:57</t>
+  </si>
+  <si>
+    <t>57.0</t>
+  </si>
+  <si>
+    <t>2010-01-21 07:54:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 16:05:19</t>
+  </si>
+  <si>
+    <t>2024-05-23 16:05:32</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>2024-05-23 16:07:32</t>
+  </si>
+  <si>
+    <t>2024-05-23 16:07:52</t>
+  </si>
+  <si>
+    <t>99556</t>
+  </si>
+  <si>
+    <t>67.0</t>
+  </si>
+  <si>
+    <t>2010-01-21 07:52:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 20:24:54</t>
+  </si>
+  <si>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>2024-05-23 21:01:00</t>
+  </si>
+  <si>
+    <t>2024-05-23 21:01:26</t>
+  </si>
+  <si>
+    <t>2024-05-23 21:01:32</t>
+  </si>
+  <si>
+    <t>71.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:32:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:32:20</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:33:32</t>
+  </si>
+  <si>
+    <t>75.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:33:52</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:34:12</t>
+  </si>
+  <si>
+    <t>77.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:34:32</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:34:52</t>
+  </si>
+  <si>
+    <t>78.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:35:12</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:35:32</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:35:52</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:36:12</t>
+  </si>
+  <si>
+    <t>81.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:36:32</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:36:52</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:37:12</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:38:25</t>
+  </si>
+  <si>
+    <t>87.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:38:45</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:39:05</t>
+  </si>
+  <si>
+    <t>88.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:39:25</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:39:45</t>
+  </si>
+  <si>
+    <t>90.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:40:05</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:40:25</t>
+  </si>
+  <si>
+    <t>91.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:40:45</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:41:05</t>
+  </si>
+  <si>
+    <t>93.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:41:25</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:41:39</t>
+  </si>
+  <si>
+    <t>94.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:44:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:44:37</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:45:00</t>
+  </si>
+  <si>
+    <t>95.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:45:20</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:45:40</t>
+  </si>
+  <si>
+    <t>97.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:48:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:48:36</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:48:57</t>
+  </si>
+  <si>
+    <t>98.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:49:17</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:49:37</t>
+  </si>
+  <si>
+    <t>99.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:49:57</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:50:00</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:55:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:55:48</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:56:09</t>
+  </si>
+  <si>
+    <t>101.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:56:29</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:56:58</t>
+  </si>
+  <si>
+    <t>103.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:57:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:57:04</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:57:25</t>
+  </si>
+  <si>
+    <t>104.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 00:57:33</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:00:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:00:49</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:01:10</t>
+  </si>
+  <si>
+    <t>106.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:01:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:01:37</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:02:05</t>
+  </si>
+  <si>
+    <t>107.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:02:14</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:02:48</t>
+  </si>
+  <si>
+    <t>109.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:08</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:10</t>
+  </si>
+  <si>
+    <t>110.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:23</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:45</t>
+  </si>
+  <si>
+    <t>111.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:03:55</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:04:03</t>
+  </si>
+  <si>
+    <t>112.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:04:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:04:59</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:14</t>
+  </si>
+  <si>
+    <t>113.0</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:00</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:19</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:25</t>
+  </si>
+  <si>
+    <t>113.5</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:27</t>
+  </si>
+  <si>
+    <t>2024-05-24 01:05:32</t>
+  </si>
+  <si>
+    <t>114.0</t>
   </si>
 </sst>
 </file>
@@ -236,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -279,13 +669,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -294,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -308,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -323,7 +713,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
@@ -337,13 +727,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -352,7 +742,7 @@
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>17</v>
@@ -366,13 +756,13 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -381,7 +771,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -395,13 +785,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -410,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
         <v>17</v>
@@ -427,10 +817,10 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -439,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
         <v>17</v>
@@ -453,13 +843,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -468,7 +858,7 @@
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
         <v>17</v>
@@ -482,13 +872,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -497,7 +887,7 @@
         <v>15</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
@@ -511,13 +901,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -526,7 +916,7 @@
         <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -540,13 +930,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -555,7 +945,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="I11" t="s">
         <v>17</v>
@@ -569,13 +959,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -584,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
@@ -598,13 +988,13 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -613,7 +1003,7 @@
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
@@ -627,22 +1017,22 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
         <v>17</v>
@@ -656,22 +1046,22 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
         <v>17</v>
@@ -685,13 +1075,13 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -700,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I16" t="s">
         <v>17</v>
@@ -714,13 +1104,13 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -729,9 +1119,1078 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" t="s">
+        <v>125</v>
+      </c>
+      <c r="I35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
+        <v>128</v>
+      </c>
+      <c r="I36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
+        <v>132</v>
+      </c>
+      <c r="I37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>135</v>
+      </c>
+      <c r="I38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" t="s">
+        <v>139</v>
+      </c>
+      <c r="I39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" t="s">
+        <v>142</v>
+      </c>
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" t="s">
+        <v>145</v>
+      </c>
+      <c r="I41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s">
+        <v>149</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" t="s">
+        <v>152</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" t="s">
+        <v>156</v>
+      </c>
+      <c r="I44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="s">
+        <v>157</v>
+      </c>
+      <c r="E45"/>
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" t="s">
+        <v>156</v>
+      </c>
+      <c r="I45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" t="s">
+        <v>161</v>
+      </c>
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" t="s">
+        <v>164</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" t="s">
+        <v>165</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" t="s">
+        <v>167</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" t="s">
+        <v>168</v>
+      </c>
+      <c r="I48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" t="s">
+        <v>171</v>
+      </c>
+      <c r="I49" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" t="s">
+        <v>175</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>176</v>
+      </c>
+      <c r="E51" t="s">
+        <v>177</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" t="s">
+        <v>178</v>
+      </c>
+      <c r="I51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" t="s">
+        <v>180</v>
+      </c>
+      <c r="E52" t="s">
+        <v>181</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" t="s">
+        <v>182</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>183</v>
+      </c>
+      <c r="D53" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" t="s">
+        <v>185</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" t="s">
+        <v>186</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" t="s">
+        <v>189</v>
+      </c>
+      <c r="I54" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>